<commit_message>
added some wiki assets, added more wine data in excels
</commit_message>
<xml_diff>
--- a/Assets/AA_Rami/research/example_wine_made_with_wine_class.xlsx
+++ b/Assets/AA_Rami/research/example_wine_made_with_wine_class.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\git_wine\wine-game\Assets\AA_Rami\research\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
   <si>
     <t>Value</t>
   </si>
@@ -35,12 +35,6 @@
     <t>Matrix</t>
   </si>
   <si>
-    <t>[scalable list of aromas]</t>
-  </si>
-  <si>
-    <t>[scalable list of flavours]</t>
-  </si>
-  <si>
     <t>Clarity</t>
   </si>
   <si>
@@ -98,15 +92,6 @@
     <t>Oak</t>
   </si>
   <si>
-    <t>DriedFruit</t>
-  </si>
-  <si>
-    <t>GreenFruit</t>
-  </si>
-  <si>
-    <t>Dairy</t>
-  </si>
-  <si>
     <t>Blossom</t>
   </si>
   <si>
@@ -116,15 +101,6 @@
     <t>Coffee</t>
   </si>
   <si>
-    <t>Raisin</t>
-  </si>
-  <si>
-    <t>RedApple</t>
-  </si>
-  <si>
-    <t>Cream</t>
-  </si>
-  <si>
     <t>Aroma[0]</t>
   </si>
   <si>
@@ -134,19 +110,7 @@
     <t>Aroma[2]</t>
   </si>
   <si>
-    <t>Flavour[0]</t>
-  </si>
-  <si>
-    <t>Flavour[1]</t>
-  </si>
-  <si>
-    <t>Flavour[2]</t>
-  </si>
-  <si>
     <t>List&lt;Int[]&gt; Aroma</t>
-  </si>
-  <si>
-    <t>List &lt;Int[]&gt; Flavours</t>
   </si>
 </sst>
 </file>
@@ -297,9 +261,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -309,6 +270,9 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -589,10 +553,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:J33"/>
+  <dimension ref="B2:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="T19" sqref="T19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -609,151 +573,151 @@
   <sheetData>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="4"/>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="F3" s="7">
+        <v>0</v>
+      </c>
+      <c r="G3" s="8">
+        <v>0</v>
+      </c>
+      <c r="H3" s="9"/>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B4" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="F4" s="11">
+        <v>1</v>
+      </c>
+      <c r="G4" s="13">
+        <v>0</v>
+      </c>
+      <c r="H4" s="14"/>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C5" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="4"/>
-      <c r="F3" s="8">
+      <c r="D5" s="4"/>
+      <c r="F5" s="7">
+        <v>2</v>
+      </c>
+      <c r="G5" s="8">
+        <v>1</v>
+      </c>
+      <c r="H5" s="9"/>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="F6" s="11">
+        <v>3</v>
+      </c>
+      <c r="G6" s="13">
+        <v>1</v>
+      </c>
+      <c r="H6" s="14"/>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="F7" s="7">
+        <v>4</v>
+      </c>
+      <c r="G7" s="8">
         <v>0</v>
       </c>
-      <c r="G3" s="9">
-        <v>0</v>
-      </c>
-      <c r="H3" s="10"/>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="12" t="s">
+      <c r="H7" s="9"/>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="4"/>
+      <c r="F8" s="11">
+        <v>5</v>
+      </c>
+      <c r="G8" s="13">
+        <v>1</v>
+      </c>
+      <c r="H8" s="14"/>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="4"/>
+      <c r="F9" s="7">
         <v>6</v>
       </c>
-      <c r="C4" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="4"/>
-      <c r="F4" s="12">
-        <v>1</v>
-      </c>
-      <c r="G4" s="14">
-        <v>0</v>
-      </c>
-      <c r="H4" s="15"/>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="8" t="s">
+      <c r="G9" s="8">
+        <v>2</v>
+      </c>
+      <c r="H9" s="9"/>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="5"/>
+      <c r="F10" s="11">
         <v>7</v>
       </c>
-      <c r="C5" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="4"/>
-      <c r="F5" s="8">
+      <c r="G10" s="13">
         <v>2</v>
       </c>
-      <c r="G5" s="9">
-        <v>1</v>
-      </c>
-      <c r="H5" s="10"/>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="4"/>
-      <c r="F6" s="12">
-        <v>3</v>
-      </c>
-      <c r="G6" s="14">
-        <v>1</v>
-      </c>
-      <c r="H6" s="15"/>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B7" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="4"/>
-      <c r="F7" s="8">
-        <v>4</v>
-      </c>
-      <c r="G7" s="9">
-        <v>0</v>
-      </c>
-      <c r="H7" s="10"/>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="4"/>
-      <c r="F8" s="12">
-        <v>5</v>
-      </c>
-      <c r="G8" s="14">
-        <v>1</v>
-      </c>
-      <c r="H8" s="15"/>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="4"/>
-      <c r="F9" s="8">
-        <v>6</v>
-      </c>
-      <c r="G9" s="9">
-        <v>2</v>
-      </c>
-      <c r="H9" s="10"/>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="5"/>
-      <c r="F10" s="12">
-        <v>7</v>
-      </c>
-      <c r="G10" s="14">
-        <v>2</v>
-      </c>
-      <c r="H10" s="15"/>
+      <c r="H10" s="14"/>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>1</v>
@@ -761,267 +725,69 @@
       <c r="D11" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F11" s="8"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="10"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="9"/>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B12" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" s="14" t="s">
+      <c r="B12" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" s="11">
+        <v>8</v>
+      </c>
+      <c r="G12" s="13">
+        <v>0</v>
+      </c>
+      <c r="H12" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="15" t="s">
+      <c r="D13" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="7">
+        <v>8</v>
+      </c>
+      <c r="G13" s="8">
+        <v>16</v>
+      </c>
+      <c r="H13" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="F12" s="12">
+      <c r="C14" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" s="11">
         <v>8</v>
       </c>
-      <c r="G12" s="14">
-        <v>0</v>
-      </c>
-      <c r="H12" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="F13" s="8">
-        <v>8</v>
-      </c>
-      <c r="G13" s="9">
-        <v>16</v>
-      </c>
-      <c r="H13" s="10">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="C14" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="D14" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="F14" s="12">
-        <v>8</v>
-      </c>
-      <c r="G14" s="14">
+      <c r="G14" s="13">
         <v>17</v>
       </c>
-      <c r="H14" s="15">
+      <c r="H14" s="14">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B15" s="8"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="10"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="10"/>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B16" s="12"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="15"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="15"/>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C17" s="9"/>
-      <c r="D17" s="10"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="10"/>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B18" s="12"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="15"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="15"/>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B19" s="8"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="10"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="10"/>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B20" s="12"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="15"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="15"/>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="8"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="10"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="10"/>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F22" s="12"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="15"/>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B23" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D23" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="F23" s="8">
-        <v>9</v>
-      </c>
-      <c r="G23" s="9">
-        <v>7</v>
-      </c>
-      <c r="H23" s="10">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B24" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="C24" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="D24" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="F24" s="12">
-        <v>9</v>
-      </c>
-      <c r="G24" s="14">
-        <v>1</v>
-      </c>
-      <c r="H24" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B25" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="D25" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="F25" s="8">
-        <v>9</v>
-      </c>
-      <c r="G25" s="9">
-        <v>15</v>
-      </c>
-      <c r="H25" s="10">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B26" s="12"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="15"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="15"/>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B27" s="8"/>
-      <c r="C27" s="9"/>
-      <c r="D27" s="10"/>
-      <c r="F27" s="8"/>
-      <c r="G27" s="9"/>
-      <c r="H27" s="10"/>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B28" s="12"/>
-      <c r="C28" s="14"/>
-      <c r="D28" s="15"/>
-      <c r="F28" s="12"/>
-      <c r="G28" s="14"/>
-      <c r="H28" s="15"/>
-    </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B29" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C29" s="9"/>
-      <c r="D29" s="10"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="9"/>
-      <c r="H29" s="10"/>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B30" s="12"/>
-      <c r="C30" s="14"/>
-      <c r="D30" s="15"/>
-      <c r="F30" s="12"/>
-      <c r="G30" s="14"/>
-      <c r="H30" s="15"/>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B31" s="8"/>
-      <c r="C31" s="9"/>
-      <c r="D31" s="10"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="9"/>
-      <c r="H31" s="10"/>
-    </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B32" s="12"/>
-      <c r="C32" s="14"/>
-      <c r="D32" s="15"/>
-      <c r="F32" s="12"/>
-      <c r="G32" s="14"/>
-      <c r="H32" s="15"/>
-    </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B33" s="8"/>
-      <c r="C33" s="9"/>
-      <c r="D33" s="10"/>
-      <c r="F33" s="8"/>
-      <c r="G33" s="9"/>
-      <c r="H33" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>